<commit_message>
rename activity names to English
</commit_message>
<xml_diff>
--- a/data/case_01.xlsx
+++ b/data/case_01.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20373"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{428CC114-0F8E-4F0B-AB64-A5800B5A7E06}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64C1BD9C-D119-4454-BF66-4F17CB54944F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,29 +20,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="11">
-  <si>
-    <t>grid</t>
-  </si>
-  <si>
-    <t>철거</t>
-  </si>
-  <si>
-    <t>마킹</t>
-  </si>
-  <si>
-    <t>칸막이A</t>
-  </si>
-  <si>
-    <t>칸막이B</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="15">
   <si>
     <t>A1</t>
   </si>
   <si>
-    <t>방통</t>
-  </si>
-  <si>
     <t>A2</t>
   </si>
   <si>
@@ -53,6 +35,46 @@
   </si>
   <si>
     <t>activity_name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>b</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>d</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>e</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>f</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>j</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>h</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>location</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -378,11 +400,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
@@ -392,146 +412,138 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
         <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" t="s">
         <v>8</v>
-      </c>
-      <c r="B12" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B14" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" t="s">
         <v>9</v>
-      </c>
-      <c r="B16" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A18" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update TODO list: 2021.05.17.
</commit_message>
<xml_diff>
--- a/data/case_01.xlsx
+++ b/data/case_01.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20373"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64C1BD9C-D119-4454-BF66-4F17CB54944F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="grid_activity_list" sheetId="1" r:id="rId1"/>
@@ -34,54 +33,54 @@
     <t>B2</t>
   </si>
   <si>
+    <t>b</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>d</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>e</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>f</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>j</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>h</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>location</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>activity_name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>b</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>a</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>c</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>d</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>e</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>a</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>f</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>j</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>h</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>location</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -399,151 +398,153 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
         <v>14</v>
       </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>3</v>
       </c>
       <c r="B14" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>3</v>
       </c>
       <c r="B16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>3</v>
       </c>
       <c r="B17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>